<commit_message>
Data fix. Small refactor. Excel data testing
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="1300" windowWidth="28800" windowHeight="17620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3900" yWindow="460" windowWidth="31060" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Table One" sheetId="1" r:id="rId1"/>
     <sheet name="Table Two" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Examples" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>string</t>
   </si>
@@ -36,59 +37,182 @@
     <t>id</t>
   </si>
   <si>
+    <t>uint</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
     <t>n</t>
   </si>
   <si>
+    <t>Name 1</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Description 1</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>is ok</t>
+  </si>
+  <si>
+    <t>Name Table 2 - 1</t>
+  </si>
+  <si>
+    <t>Description Table 2 - 2</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>Byte Value</t>
+  </si>
+  <si>
+    <t>sbyte</t>
+  </si>
+  <si>
+    <t>sb</t>
+  </si>
+  <si>
+    <t>Signed Byte Value</t>
+  </si>
+  <si>
+    <t>Int Value</t>
+  </si>
+  <si>
+    <t>ui</t>
+  </si>
+  <si>
+    <t>Unsigned Int Value</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>Short Value</t>
+  </si>
+  <si>
+    <t>ushort</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>Unsigned Short Value</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
     <t>l</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>lenght</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>uint</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>byte</t>
-  </si>
-  <si>
-    <t>io</t>
-  </si>
-  <si>
-    <t>cr</t>
-  </si>
-  <si>
-    <t>cg</t>
-  </si>
-  <si>
-    <t>cb</t>
-  </si>
-  <si>
-    <t>is_ok</t>
-  </si>
-  <si>
-    <t>color_red</t>
-  </si>
-  <si>
-    <t>color_green</t>
-  </si>
-  <si>
-    <t>color_blue</t>
+    <t>Long Value</t>
+  </si>
+  <si>
+    <t>ulong</t>
+  </si>
+  <si>
+    <t>ul</t>
+  </si>
+  <si>
+    <t>Unsigned Long Value</t>
+  </si>
+  <si>
+    <t>Float Value</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>Double Value</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Char Value</t>
+  </si>
+  <si>
+    <t>bo</t>
+  </si>
+  <si>
+    <t>Boolean Value</t>
+  </si>
+  <si>
+    <t>st</t>
+  </si>
+  <si>
+    <t>String Value</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t>Decimal Value</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Name 2</t>
+  </si>
+  <si>
+    <t>Description 2</t>
+  </si>
+  <si>
+    <t>Name 3</t>
+  </si>
+  <si>
+    <t>Description 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -103,8 +227,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +244,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -130,10 +265,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -413,57 +554,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1.55</v>
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>1999</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>2015</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6">
+        <v>2014</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -473,81 +672,271 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="b">
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
-        <v>255</v>
-      </c>
-      <c r="D4" s="1">
-        <v>255</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
         <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>-2</v>
+      </c>
+      <c r="C4">
+        <v>-123456</v>
+      </c>
+      <c r="D4">
+        <v>123456</v>
+      </c>
+      <c r="E4">
+        <v>-64</v>
+      </c>
+      <c r="F4">
+        <v>64</v>
+      </c>
+      <c r="G4">
+        <v>-123456789</v>
+      </c>
+      <c r="H4">
+        <v>12345679</v>
+      </c>
+      <c r="I4">
+        <v>1.2344999999999999</v>
+      </c>
+      <c r="J4">
+        <v>1.2345678899999999</v>
+      </c>
+      <c r="K4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>0.222222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for ignoring sheets
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsilva/Workspace/Transformo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanssl/Workspace/Transformo/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="1760" windowWidth="22360" windowHeight="15800" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4700" yWindow="1760" windowWidth="22360" windowHeight="15800" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" r:id="rId1"/>
     <sheet name="Category Has Image" sheetId="3" r:id="rId2"/>
     <sheet name="Image" sheetId="2" r:id="rId3"/>
+    <sheet name="!Comments" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="131">
   <si>
     <t>ushort</t>
   </si>
@@ -395,6 +396,30 @@
   </si>
   <si>
     <t>id@</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>The category table contains the code and description of the weather</t>
+  </si>
+  <si>
+    <t>Category has Image</t>
+  </si>
+  <si>
+    <t>Contains the link between images and Category</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Represent an image depicting a weather condition</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -1726,7 +1751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2091,4 +2116,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>